<commit_message>
Add tools for tools like obtenerArchivoOrigen
</commit_message>
<xml_diff>
--- a/girlsFull.xlsx
+++ b/girlsFull.xlsx
@@ -1777,7 +1777,11 @@
           <t>3quarters-mediumshot.jfif</t>
         </is>
       </c>
-      <c r="T15" t="inlineStr"/>
+      <c r="T15" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\14-t2.jfif</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1798,7 +1802,11 @@
           <t>14-t3.jfif</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr"/>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F16" t="inlineStr">
         <is>
           <t>in leather</t>
@@ -1861,7 +1869,11 @@
           <t>front-mediumshot2.png</t>
         </is>
       </c>
-      <c r="T16" t="inlineStr"/>
+      <c r="T16" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\14-t3.jfif</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1882,7 +1894,11 @@
           <t>14-t4.jfif</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr"/>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr"/>
@@ -1937,7 +1953,11 @@
           <t>front-mediumshot1.png</t>
         </is>
       </c>
-      <c r="T17" t="inlineStr"/>
+      <c r="T17" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\14-t4.jfif</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1958,7 +1978,11 @@
           <t>15-t1.webp</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr"/>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F18" t="inlineStr">
         <is>
           <t>hot</t>
@@ -2017,7 +2041,11 @@
           <t>face.jpg</t>
         </is>
       </c>
-      <c r="T18" t="inlineStr"/>
+      <c r="T18" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\15-t1.webp</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2038,7 +2066,11 @@
           <t>15-t2.webp</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr"/>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F19" t="inlineStr">
         <is>
           <t>provocative</t>
@@ -2109,7 +2141,11 @@
           <t>front-mediumshot8.jpg</t>
         </is>
       </c>
-      <c r="T19" t="inlineStr"/>
+      <c r="T19" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\15-t2.webp</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2130,7 +2166,11 @@
           <t>15-t3.webp</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr"/>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F20" t="inlineStr">
         <is>
           <t>sensual</t>
@@ -2193,7 +2233,11 @@
           <t>stand-handhead.jpg</t>
         </is>
       </c>
-      <c r="T20" t="inlineStr"/>
+      <c r="T20" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\15-t3.webp</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2214,7 +2258,11 @@
           <t>15-t4.webp</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr"/>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F21" t="inlineStr">
         <is>
           <t>beautiful</t>
@@ -2273,7 +2321,11 @@
           <t>handsup.jpg</t>
         </is>
       </c>
-      <c r="T21" t="inlineStr"/>
+      <c r="T21" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\15-t4.webp</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2294,7 +2346,11 @@
           <t>1520115753422-t1.jpg</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr"/>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F22" t="inlineStr">
         <is>
           <t>beautiful</t>
@@ -2353,7 +2409,11 @@
           <t>stand-far.jpg</t>
         </is>
       </c>
-      <c r="T22" t="inlineStr"/>
+      <c r="T22" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\1520115753422-t1.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2374,7 +2434,11 @@
           <t>1520115753422-t2.jpg</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr"/>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="inlineStr">
         <is>
@@ -2437,7 +2501,11 @@
           <t>double.jpg</t>
         </is>
       </c>
-      <c r="T23" t="inlineStr"/>
+      <c r="T23" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\1520115753422-t2.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2458,7 +2526,11 @@
           <t>1520115753422-t3.jpg</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr"/>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F24" t="inlineStr">
         <is>
           <t>hot</t>
@@ -2525,7 +2597,11 @@
           <t>front-mediumshot.png</t>
         </is>
       </c>
-      <c r="T24" t="inlineStr"/>
+      <c r="T24" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\1520115753422-t3.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2546,7 +2622,11 @@
           <t>1520115753422-t4.jpg</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr"/>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr">
@@ -2601,7 +2681,11 @@
           <t>hands-waist.webp</t>
         </is>
       </c>
-      <c r="T25" t="inlineStr"/>
+      <c r="T25" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\1520115753422-t4.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">

</xml_diff>

<commit_message>
Separación de creación de columna de imagenes
</commit_message>
<xml_diff>
--- a/girlsFull.xlsx
+++ b/girlsFull.xlsx
@@ -3882,7 +3882,11 @@
           <t>4-t2.jpg</t>
         </is>
       </c>
-      <c r="E39" t="inlineStr"/>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F39" t="inlineStr">
         <is>
           <t>provocative</t>
@@ -3937,7 +3941,11 @@
           <t>legscrossed.jpg</t>
         </is>
       </c>
-      <c r="T39" t="inlineStr"/>
+      <c r="T39" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\4-t2.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -3958,7 +3966,11 @@
           <t>4-t3.jpg</t>
         </is>
       </c>
-      <c r="E40" t="inlineStr"/>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F40" t="inlineStr">
         <is>
           <t>in leather</t>
@@ -4021,7 +4033,11 @@
           <t>halfbody-handswaist.webp</t>
         </is>
       </c>
-      <c r="T40" t="inlineStr"/>
+      <c r="T40" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\4-t3.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -4101,7 +4117,11 @@
           <t>front-americanshot.jpg</t>
         </is>
       </c>
-      <c r="T41" t="inlineStr"/>
+      <c r="T41" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\4-t4.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -4122,7 +4142,11 @@
           <t>5-t1.jpg</t>
         </is>
       </c>
-      <c r="E42" t="inlineStr"/>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F42" t="inlineStr"/>
       <c r="G42" t="inlineStr">
         <is>
@@ -4185,7 +4209,11 @@
           <t>dancing.jpg</t>
         </is>
       </c>
-      <c r="T42" t="inlineStr"/>
+      <c r="T42" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\5-t1.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -4206,7 +4234,11 @@
           <t>5-t2.jpg</t>
         </is>
       </c>
-      <c r="E43" t="inlineStr"/>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F43" t="inlineStr"/>
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr"/>
@@ -4261,7 +4293,11 @@
           <t>front-mediumshot4.png</t>
         </is>
       </c>
-      <c r="T43" t="inlineStr"/>
+      <c r="T43" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\5-t2.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -4282,7 +4318,11 @@
           <t>5-t3.jpg</t>
         </is>
       </c>
-      <c r="E44" t="inlineStr"/>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F44" t="inlineStr">
         <is>
           <t>beautiful</t>
@@ -4345,7 +4385,11 @@
           <t>hands-behind-head.webp</t>
         </is>
       </c>
-      <c r="T44" t="inlineStr"/>
+      <c r="T44" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\5-t3.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -4366,7 +4410,11 @@
           <t>5-t4.jpg</t>
         </is>
       </c>
-      <c r="E45" t="inlineStr"/>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F45" t="inlineStr"/>
       <c r="G45" t="inlineStr"/>
       <c r="H45" t="inlineStr">
@@ -4425,7 +4473,11 @@
           <t>stand-profile-2.jpg</t>
         </is>
       </c>
-      <c r="T45" t="inlineStr"/>
+      <c r="T45" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\5-t4.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -4446,7 +4498,11 @@
           <t>6-t1.jpg</t>
         </is>
       </c>
-      <c r="E46" t="inlineStr"/>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F46" t="inlineStr">
         <is>
           <t>beautiful</t>
@@ -4513,7 +4569,11 @@
           <t>front-mediumshot.jpg</t>
         </is>
       </c>
-      <c r="T46" t="inlineStr"/>
+      <c r="T46" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\6-t1.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -4534,7 +4594,11 @@
           <t>6-t2.jpg</t>
         </is>
       </c>
-      <c r="E47" t="inlineStr"/>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F47" t="inlineStr">
         <is>
           <t>provocative</t>
@@ -4593,7 +4657,11 @@
           <t>front-mediumshot.png</t>
         </is>
       </c>
-      <c r="T47" t="inlineStr"/>
+      <c r="T47" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\6-t2.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -4614,7 +4682,11 @@
           <t>6-t3.jpg</t>
         </is>
       </c>
-      <c r="E48" t="inlineStr"/>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F48" t="inlineStr">
         <is>
           <t>provocative</t>
@@ -4673,7 +4745,11 @@
           <t>3q-stand-legswide.jpeg</t>
         </is>
       </c>
-      <c r="T48" t="inlineStr"/>
+      <c r="T48" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\6-t3.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -4694,7 +4770,11 @@
           <t>6-t4.jpg</t>
         </is>
       </c>
-      <c r="E49" t="inlineStr"/>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F49" t="inlineStr">
         <is>
           <t>sensual</t>
@@ -4757,7 +4837,11 @@
           <t>3quarters-arms-up.jpg</t>
         </is>
       </c>
-      <c r="T49" t="inlineStr"/>
+      <c r="T49" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\6-t4.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -4778,7 +4862,11 @@
           <t>7-t1.jpg</t>
         </is>
       </c>
-      <c r="E50" t="inlineStr"/>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 'Cannot find any face in the reference image! Please upload another person image'</t>
+        </is>
+      </c>
       <c r="F50" t="inlineStr">
         <is>
           <t>sensual</t>
@@ -4858,7 +4946,11 @@
           <t>7-t2.jpg</t>
         </is>
       </c>
-      <c r="E51" t="inlineStr"/>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F51" t="inlineStr">
         <is>
           <t>provocative</t>
@@ -4921,7 +5013,11 @@
           <t>stand-lookup.jpg</t>
         </is>
       </c>
-      <c r="T51" t="inlineStr"/>
+      <c r="T51" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\7-t2.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -4942,7 +5038,11 @@
           <t>7-t3.jpg</t>
         </is>
       </c>
-      <c r="E52" t="inlineStr"/>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F52" t="inlineStr"/>
       <c r="G52" t="inlineStr">
         <is>
@@ -4997,7 +5097,11 @@
           <t>face.jpg</t>
         </is>
       </c>
-      <c r="T52" t="inlineStr"/>
+      <c r="T52" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\7-t3.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -5018,7 +5122,11 @@
           <t>7-t4.jpg</t>
         </is>
       </c>
-      <c r="E53" t="inlineStr"/>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F53" t="inlineStr">
         <is>
           <t>in leather</t>
@@ -5081,7 +5189,11 @@
           <t>stand-stretch.jpg</t>
         </is>
       </c>
-      <c r="T53" t="inlineStr"/>
+      <c r="T53" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\7-t4.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -5102,7 +5214,11 @@
           <t>9-t1.jpg</t>
         </is>
       </c>
-      <c r="E54" t="inlineStr"/>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F54" t="inlineStr">
         <is>
           <t>provocative</t>
@@ -5169,7 +5285,11 @@
           <t>front-mediumshot7.png</t>
         </is>
       </c>
-      <c r="T54" t="inlineStr"/>
+      <c r="T54" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\9-t1.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -5190,7 +5310,11 @@
           <t>9-t2.jpg</t>
         </is>
       </c>
-      <c r="E55" t="inlineStr"/>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F55" t="inlineStr"/>
       <c r="G55" t="inlineStr"/>
       <c r="H55" t="inlineStr">
@@ -5249,7 +5373,11 @@
           <t>flying-pointing.jpg</t>
         </is>
       </c>
-      <c r="T55" t="inlineStr"/>
+      <c r="T55" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\9-t2.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -5270,7 +5398,11 @@
           <t>9-t3.jpg</t>
         </is>
       </c>
-      <c r="E56" t="inlineStr"/>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F56" t="inlineStr">
         <is>
           <t>in leather</t>
@@ -5333,7 +5465,11 @@
           <t>front-mediumshot3.png</t>
         </is>
       </c>
-      <c r="T56" t="inlineStr"/>
+      <c r="T56" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\9-t3.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -5354,7 +5490,11 @@
           <t>9-t4.jpg</t>
         </is>
       </c>
-      <c r="E57" t="inlineStr"/>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F57" t="inlineStr">
         <is>
           <t>hot</t>
@@ -5413,7 +5553,11 @@
           <t>arms-shoulder.jpg</t>
         </is>
       </c>
-      <c r="T57" t="inlineStr"/>
+      <c r="T57" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\9-t4.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -5434,7 +5578,11 @@
           <t>9238727-t1.jpg</t>
         </is>
       </c>
-      <c r="E58" t="inlineStr"/>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F58" t="inlineStr"/>
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="inlineStr"/>
@@ -5489,7 +5637,11 @@
           <t>profile-mediumshot.jpg</t>
         </is>
       </c>
-      <c r="T58" t="inlineStr"/>
+      <c r="T58" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\9238727-t1.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -5510,7 +5662,11 @@
           <t>9238727-t2.jpg</t>
         </is>
       </c>
-      <c r="E59" t="inlineStr"/>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F59" t="inlineStr"/>
       <c r="G59" t="inlineStr">
         <is>
@@ -5557,7 +5713,11 @@
           <t>stand-armscrossed.jpg</t>
         </is>
       </c>
-      <c r="T59" t="inlineStr"/>
+      <c r="T59" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\9238727-t2.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -5578,7 +5738,11 @@
           <t>9238727-t3.jpg</t>
         </is>
       </c>
-      <c r="E60" t="inlineStr"/>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F60" t="inlineStr"/>
       <c r="G60" t="inlineStr"/>
       <c r="H60" t="inlineStr"/>
@@ -5633,7 +5797,11 @@
           <t>3q-stand-legswide.jpeg</t>
         </is>
       </c>
-      <c r="T60" t="inlineStr"/>
+      <c r="T60" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\9238727-t3.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -5654,7 +5822,11 @@
           <t>9238727-t4.jpg</t>
         </is>
       </c>
-      <c r="E61" t="inlineStr"/>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F61" t="inlineStr">
         <is>
           <t>hot</t>
@@ -5717,7 +5889,11 @@
           <t>hand-in-chest.webp</t>
         </is>
       </c>
-      <c r="T61" t="inlineStr"/>
+      <c r="T61" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\9238727-t4.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -5738,7 +5914,11 @@
           <t>A-Ruby-Young-t1.png</t>
         </is>
       </c>
-      <c r="E62" t="inlineStr"/>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F62" t="inlineStr">
         <is>
           <t>hot</t>
@@ -5801,7 +5981,11 @@
           <t>front-mediumshot3.png</t>
         </is>
       </c>
-      <c r="T62" t="inlineStr"/>
+      <c r="T62" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\A-Ruby-Young-t1.png</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -5822,7 +6006,11 @@
           <t>A-Ruby-Young-t2.png</t>
         </is>
       </c>
-      <c r="E63" t="inlineStr"/>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F63" t="inlineStr">
         <is>
           <t>naughty</t>
@@ -5881,7 +6069,11 @@
           <t>pose.jpg</t>
         </is>
       </c>
-      <c r="T63" t="inlineStr"/>
+      <c r="T63" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\A-Ruby-Young-t2.png</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -5902,7 +6094,11 @@
           <t>A-Ruby-Young-t3.png</t>
         </is>
       </c>
-      <c r="E64" t="inlineStr"/>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F64" t="inlineStr">
         <is>
           <t>beautiful</t>
@@ -5969,7 +6165,11 @@
           <t>group.jpg</t>
         </is>
       </c>
-      <c r="T64" t="inlineStr"/>
+      <c r="T64" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\A-Ruby-Young-t3.png</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -5990,7 +6190,11 @@
           <t>A-Ruby-Young-t4.png</t>
         </is>
       </c>
-      <c r="E65" t="inlineStr"/>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F65" t="inlineStr"/>
       <c r="G65" t="inlineStr">
         <is>
@@ -6053,7 +6257,11 @@
           <t>olympian.jpg</t>
         </is>
       </c>
-      <c r="T65" t="inlineStr"/>
+      <c r="T65" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\A-Ruby-Young-t4.png</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -6074,7 +6282,11 @@
           <t>Albanese-t1.jpg</t>
         </is>
       </c>
-      <c r="E66" t="inlineStr"/>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F66" t="inlineStr">
         <is>
           <t>beautiful</t>
@@ -6133,7 +6345,11 @@
           <t>stand-lookup.jpg</t>
         </is>
       </c>
-      <c r="T66" t="inlineStr"/>
+      <c r="T66" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\Albanese-t1.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -6154,7 +6370,11 @@
           <t>Albanese-t2.jpg</t>
         </is>
       </c>
-      <c r="E67" t="inlineStr"/>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 'Cannot find any face in the reference image! Please upload another person image'</t>
+        </is>
+      </c>
       <c r="F67" t="inlineStr">
         <is>
           <t>in leather</t>
@@ -6230,7 +6450,11 @@
           <t>Albanese-t3.jpg</t>
         </is>
       </c>
-      <c r="E68" t="inlineStr"/>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F68" t="inlineStr">
         <is>
           <t>naughty</t>
@@ -6289,7 +6513,11 @@
           <t>front-americanshot1.jpg</t>
         </is>
       </c>
-      <c r="T68" t="inlineStr"/>
+      <c r="T68" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\Albanese-t3.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -6310,7 +6538,11 @@
           <t>Albanese-t4.jpg</t>
         </is>
       </c>
-      <c r="E69" t="inlineStr"/>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F69" t="inlineStr"/>
       <c r="G69" t="inlineStr">
         <is>
@@ -6365,7 +6597,11 @@
           <t>stretch.jpg</t>
         </is>
       </c>
-      <c r="T69" t="inlineStr"/>
+      <c r="T69" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\Albanese-t4.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -6386,7 +6622,11 @@
           <t>AleCaballeroCreadoraDigital-t1.jpg</t>
         </is>
       </c>
-      <c r="E70" t="inlineStr"/>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F70" t="inlineStr"/>
       <c r="G70" t="inlineStr">
         <is>
@@ -6445,7 +6685,11 @@
           <t>stand-handhead.jpg</t>
         </is>
       </c>
-      <c r="T70" t="inlineStr"/>
+      <c r="T70" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\AleCaballeroCreadoraDigital-t1.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -6466,7 +6710,11 @@
           <t>AleCaballeroCreadoraDigital-t2.jpg</t>
         </is>
       </c>
-      <c r="E71" t="inlineStr"/>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F71" t="inlineStr">
         <is>
           <t>beautiful</t>
@@ -6533,7 +6781,11 @@
           <t>pop.png</t>
         </is>
       </c>
-      <c r="T71" t="inlineStr"/>
+      <c r="T71" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\AleCaballeroCreadoraDigital-t2.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -6554,7 +6806,11 @@
           <t>AleCaballeroCreadoraDigital-t3.jpg</t>
         </is>
       </c>
-      <c r="E72" t="inlineStr"/>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F72" t="inlineStr">
         <is>
           <t>hot</t>
@@ -6625,7 +6881,11 @@
           <t>3quarters-mediumshot2.png</t>
         </is>
       </c>
-      <c r="T72" t="inlineStr"/>
+      <c r="T72" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\AleCaballeroCreadoraDigital-t3.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -6646,7 +6906,11 @@
           <t>AleCaballeroCreadoraDigital-t4.jpg</t>
         </is>
       </c>
-      <c r="E73" t="inlineStr"/>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F73" t="inlineStr">
         <is>
           <t>sensual</t>
@@ -6709,7 +6973,11 @@
           <t>squat.jpg</t>
         </is>
       </c>
-      <c r="T73" t="inlineStr"/>
+      <c r="T73" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\AleCaballeroCreadoraDigital-t4.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -6730,7 +6998,11 @@
           <t>AlejMolina-t1.jpg</t>
         </is>
       </c>
-      <c r="E74" t="inlineStr"/>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F74" t="inlineStr"/>
       <c r="G74" t="inlineStr"/>
       <c r="H74" t="inlineStr">
@@ -6789,7 +7061,11 @@
           <t>weights-armsup.webp</t>
         </is>
       </c>
-      <c r="T74" t="inlineStr"/>
+      <c r="T74" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\AlejMolina-t1.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -6810,7 +7086,11 @@
           <t>AlejMolina-t2.jpg</t>
         </is>
       </c>
-      <c r="E75" t="inlineStr"/>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F75" t="inlineStr"/>
       <c r="G75" t="inlineStr">
         <is>
@@ -6877,7 +7157,11 @@
           <t>3quarters-mediumshot.jpg</t>
         </is>
       </c>
-      <c r="T75" t="inlineStr"/>
+      <c r="T75" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\AlejMolina-t2.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -6898,7 +7182,11 @@
           <t>AlejMolina-t3.jpg</t>
         </is>
       </c>
-      <c r="E76" t="inlineStr"/>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F76" t="inlineStr">
         <is>
           <t>naughty</t>
@@ -6957,7 +7245,11 @@
           <t>front-mediumshot9.png</t>
         </is>
       </c>
-      <c r="T76" t="inlineStr"/>
+      <c r="T76" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\AlejMolina-t3.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -6978,7 +7270,11 @@
           <t>AlejMolina-t4.jpg</t>
         </is>
       </c>
-      <c r="E77" t="inlineStr"/>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F77" t="inlineStr">
         <is>
           <t>hot</t>
@@ -7045,7 +7341,11 @@
           <t>front-mediumdownshot.png</t>
         </is>
       </c>
-      <c r="T77" t="inlineStr"/>
+      <c r="T77" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\AlejMolina-t4.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -7066,7 +7366,11 @@
           <t>AlejandraMolina-t1.jpeg</t>
         </is>
       </c>
-      <c r="E78" t="inlineStr"/>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F78" t="inlineStr">
         <is>
           <t>beautiful</t>
@@ -7121,7 +7425,11 @@
           <t>handup-2.jpg</t>
         </is>
       </c>
-      <c r="T78" t="inlineStr"/>
+      <c r="T78" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\AlejandraMolina-t1.jpeg</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -7142,7 +7450,11 @@
           <t>AlejandraMolina-t2.jpeg</t>
         </is>
       </c>
-      <c r="E79" t="inlineStr"/>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F79" t="inlineStr">
         <is>
           <t>naughty</t>
@@ -7201,7 +7513,11 @@
           <t>dancing.jpg</t>
         </is>
       </c>
-      <c r="T79" t="inlineStr"/>
+      <c r="T79" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\AlejandraMolina-t2.jpeg</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -7222,7 +7538,11 @@
           <t>AlejandraMolina-t3.jpeg</t>
         </is>
       </c>
-      <c r="E80" t="inlineStr"/>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F80" t="inlineStr"/>
       <c r="G80" t="inlineStr">
         <is>
@@ -7281,7 +7601,11 @@
           <t>3quarters-mediumshot3.png</t>
         </is>
       </c>
-      <c r="T80" t="inlineStr"/>
+      <c r="T80" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\AlejandraMolina-t3.jpeg</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -7302,7 +7626,11 @@
           <t>AlejandraMolina-t4.jpeg</t>
         </is>
       </c>
-      <c r="E81" t="inlineStr"/>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F81" t="inlineStr"/>
       <c r="G81" t="inlineStr"/>
       <c r="H81" t="inlineStr">
@@ -7361,7 +7689,11 @@
           <t>3quarters-mediumshotdown.jfif</t>
         </is>
       </c>
-      <c r="T81" t="inlineStr"/>
+      <c r="T81" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\AlejandraMolina-t4.jpeg</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -7412,7 +7744,11 @@
           <t>AnaKournikova-t1.png</t>
         </is>
       </c>
-      <c r="E83" t="inlineStr"/>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F83" t="inlineStr">
         <is>
           <t>naughty</t>
@@ -7479,7 +7815,11 @@
           <t>front-mediumshot9.jpg</t>
         </is>
       </c>
-      <c r="T83" t="inlineStr"/>
+      <c r="T83" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\AnaKournikova-t1.png</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -7500,7 +7840,11 @@
           <t>AnaKournikova-t2.png</t>
         </is>
       </c>
-      <c r="E84" t="inlineStr"/>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F84" t="inlineStr"/>
       <c r="G84" t="inlineStr">
         <is>
@@ -7559,7 +7903,11 @@
           <t>3q-stand-legswide.jpeg</t>
         </is>
       </c>
-      <c r="T84" t="inlineStr"/>
+      <c r="T84" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\AnaKournikova-t2.png</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -7580,7 +7928,11 @@
           <t>AnaKournikova-t3.png</t>
         </is>
       </c>
-      <c r="E85" t="inlineStr"/>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F85" t="inlineStr">
         <is>
           <t>in leather</t>
@@ -7643,7 +7995,11 @@
           <t>handup.jpg</t>
         </is>
       </c>
-      <c r="T85" t="inlineStr"/>
+      <c r="T85" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\AnaKournikova-t3.png</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -7664,7 +8020,11 @@
           <t>AnaKournikova-t4.png</t>
         </is>
       </c>
-      <c r="E86" t="inlineStr"/>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F86" t="inlineStr">
         <is>
           <t>provocative</t>
@@ -7731,7 +8091,11 @@
           <t>sitting.jpg</t>
         </is>
       </c>
-      <c r="T86" t="inlineStr"/>
+      <c r="T86" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\AnaKournikova-t4.png</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -7752,7 +8116,11 @@
           <t>Anahí-t1.png</t>
         </is>
       </c>
-      <c r="E87" t="inlineStr"/>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F87" t="inlineStr">
         <is>
           <t>beautiful</t>
@@ -7807,7 +8175,11 @@
           <t>group.jpg</t>
         </is>
       </c>
-      <c r="T87" t="inlineStr"/>
+      <c r="T87" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\Anahí-t1.png</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -7828,7 +8200,11 @@
           <t>Anahí-t2.png</t>
         </is>
       </c>
-      <c r="E88" t="inlineStr"/>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F88" t="inlineStr">
         <is>
           <t>provocative</t>
@@ -7895,7 +8271,11 @@
           <t>stand-profile.jpg</t>
         </is>
       </c>
-      <c r="T88" t="inlineStr"/>
+      <c r="T88" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\Anahí-t2.png</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -7916,7 +8296,11 @@
           <t>Anahí-t3.png</t>
         </is>
       </c>
-      <c r="E89" t="inlineStr"/>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F89" t="inlineStr">
         <is>
           <t>naughty</t>
@@ -7979,7 +8363,11 @@
           <t>duck-handup.jpg</t>
         </is>
       </c>
-      <c r="T89" t="inlineStr"/>
+      <c r="T89" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\Anahí-t3.png</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -8000,7 +8388,11 @@
           <t>Anahí-t4.png</t>
         </is>
       </c>
-      <c r="E90" t="inlineStr"/>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F90" t="inlineStr"/>
       <c r="G90" t="inlineStr"/>
       <c r="H90" t="inlineStr"/>
@@ -8043,7 +8435,11 @@
           <t>stand-profile.jpg</t>
         </is>
       </c>
-      <c r="T90" t="inlineStr"/>
+      <c r="T90" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\Anahí-t4.png</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -8064,7 +8460,11 @@
           <t>AnaisTorres-t1.jpg</t>
         </is>
       </c>
-      <c r="E91" t="inlineStr"/>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F91" t="inlineStr"/>
       <c r="G91" t="inlineStr"/>
       <c r="H91" t="inlineStr"/>
@@ -8123,7 +8523,11 @@
           <t>3quarters-mediumshot6.png</t>
         </is>
       </c>
-      <c r="T91" t="inlineStr"/>
+      <c r="T91" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\AnaisTorres-t1.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -8144,7 +8548,11 @@
           <t>AnaisTorres-t2.jpg</t>
         </is>
       </c>
-      <c r="E92" t="inlineStr"/>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F92" t="inlineStr"/>
       <c r="G92" t="inlineStr"/>
       <c r="H92" t="inlineStr">
@@ -8203,7 +8611,11 @@
           <t>arm-up.jpg</t>
         </is>
       </c>
-      <c r="T92" t="inlineStr"/>
+      <c r="T92" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\AnaisTorres-t2.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -8224,7 +8636,11 @@
           <t>AnaisTorres-t3.jpg</t>
         </is>
       </c>
-      <c r="E93" t="inlineStr"/>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F93" t="inlineStr">
         <is>
           <t>sensual</t>
@@ -8283,7 +8699,11 @@
           <t>front-mediumshot.jfif</t>
         </is>
       </c>
-      <c r="T93" t="inlineStr"/>
+      <c r="T93" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\AnaisTorres-t3.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -8304,7 +8724,11 @@
           <t>AnaisTorres-t4.jpg</t>
         </is>
       </c>
-      <c r="E94" t="inlineStr"/>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F94" t="inlineStr"/>
       <c r="G94" t="inlineStr">
         <is>
@@ -8351,7 +8775,11 @@
           <t>hands-behind-head.webp</t>
         </is>
       </c>
-      <c r="T94" t="inlineStr"/>
+      <c r="T94" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\AnaisTorres-t4.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -8372,7 +8800,11 @@
           <t>Anny-t1.jpg</t>
         </is>
       </c>
-      <c r="E95" t="inlineStr"/>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F95" t="inlineStr">
         <is>
           <t>provocative</t>
@@ -8435,7 +8867,11 @@
           <t>stretch.jpg</t>
         </is>
       </c>
-      <c r="T95" t="inlineStr"/>
+      <c r="T95" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\Anny-t1.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -8456,7 +8892,11 @@
           <t>Anny-t2.jpg</t>
         </is>
       </c>
-      <c r="E96" t="inlineStr"/>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F96" t="inlineStr">
         <is>
           <t>naughty</t>
@@ -8523,7 +8963,11 @@
           <t>3quarters-mediumshot5.png</t>
         </is>
       </c>
-      <c r="T96" t="inlineStr"/>
+      <c r="T96" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\Anny-t2.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -8544,7 +8988,11 @@
           <t>Anny-t3.jpg</t>
         </is>
       </c>
-      <c r="E97" t="inlineStr"/>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F97" t="inlineStr">
         <is>
           <t>in leather</t>
@@ -8607,7 +9055,11 @@
           <t>3quarters-mediumshot3.png</t>
         </is>
       </c>
-      <c r="T97" t="inlineStr"/>
+      <c r="T97" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\Anny-t3.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -8628,7 +9080,11 @@
           <t>Anny-t4.jpg</t>
         </is>
       </c>
-      <c r="E98" t="inlineStr"/>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F98" t="inlineStr">
         <is>
           <t>sensual</t>
@@ -8687,7 +9143,11 @@
           <t>face.jpg</t>
         </is>
       </c>
-      <c r="T98" t="inlineStr"/>
+      <c r="T98" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\Anny-t4.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -8708,7 +9168,11 @@
           <t>AnyPokimane-t1.webp</t>
         </is>
       </c>
-      <c r="E99" t="inlineStr"/>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F99" t="inlineStr">
         <is>
           <t>in leather</t>
@@ -8763,7 +9227,11 @@
           <t>front-mediumshot7.png</t>
         </is>
       </c>
-      <c r="T99" t="inlineStr"/>
+      <c r="T99" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\AnyPokimane-t1.webp</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -8784,7 +9252,11 @@
           <t>AnyPokimane-t2.webp</t>
         </is>
       </c>
-      <c r="E100" t="inlineStr"/>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F100" t="inlineStr">
         <is>
           <t>hot</t>
@@ -8843,7 +9315,11 @@
           <t>stand-profile.jpg</t>
         </is>
       </c>
-      <c r="T100" t="inlineStr"/>
+      <c r="T100" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\AnyPokimane-t2.webp</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -8864,7 +9340,11 @@
           <t>AnyPokimane-t3.webp</t>
         </is>
       </c>
-      <c r="E101" t="inlineStr"/>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F101" t="inlineStr">
         <is>
           <t>provocative</t>
@@ -8931,7 +9411,11 @@
           <t>front-mediumshot1.png</t>
         </is>
       </c>
-      <c r="T101" t="inlineStr"/>
+      <c r="T101" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\AnyPokimane-t3.webp</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -8952,7 +9436,11 @@
           <t>AnyPokimane-t4.webp</t>
         </is>
       </c>
-      <c r="E102" t="inlineStr"/>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F102" t="inlineStr">
         <is>
           <t>provocative</t>
@@ -9015,7 +9503,11 @@
           <t>3quarters-mediumshot.jpg</t>
         </is>
       </c>
-      <c r="T102" t="inlineStr"/>
+      <c r="T102" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\AnyPokimane-t4.webp</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -9036,7 +9528,11 @@
           <t>Art-t1.png</t>
         </is>
       </c>
-      <c r="E103" t="inlineStr"/>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F103" t="inlineStr">
         <is>
           <t>in leather</t>
@@ -9099,7 +9595,11 @@
           <t>3quarters-mediumshot5.png</t>
         </is>
       </c>
-      <c r="T103" t="inlineStr"/>
+      <c r="T103" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\Art-t1.png</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -9120,7 +9620,11 @@
           <t>Art-t2.png</t>
         </is>
       </c>
-      <c r="E104" t="inlineStr"/>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F104" t="inlineStr">
         <is>
           <t>beautiful</t>
@@ -9179,7 +9683,11 @@
           <t>front-mediumshot.png</t>
         </is>
       </c>
-      <c r="T104" t="inlineStr"/>
+      <c r="T104" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\Art-t2.png</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -9200,7 +9708,11 @@
           <t>Art-t3.png</t>
         </is>
       </c>
-      <c r="E105" t="inlineStr"/>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F105" t="inlineStr">
         <is>
           <t>provocative</t>
@@ -9263,7 +9775,11 @@
           <t>far-fullbody.jpg</t>
         </is>
       </c>
-      <c r="T105" t="inlineStr"/>
+      <c r="T105" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\Art-t3.png</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -9284,7 +9800,11 @@
           <t>Art-t4.png</t>
         </is>
       </c>
-      <c r="E106" t="inlineStr"/>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F106" t="inlineStr">
         <is>
           <t>in leather</t>
@@ -9347,7 +9867,11 @@
           <t>handup.jpg</t>
         </is>
       </c>
-      <c r="T106" t="inlineStr"/>
+      <c r="T106" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\Art-t4.png</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -9368,7 +9892,11 @@
           <t>Beautiful-Deepika-Padukone-t1.jpg</t>
         </is>
       </c>
-      <c r="E107" t="inlineStr"/>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F107" t="inlineStr"/>
       <c r="G107" t="inlineStr">
         <is>
@@ -9431,7 +9959,11 @@
           <t>3quarters-mediumshotdown.webp</t>
         </is>
       </c>
-      <c r="T107" t="inlineStr"/>
+      <c r="T107" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\Beautiful-Deepika-Padukone-t1.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -9452,7 +9984,11 @@
           <t>Beautiful-Deepika-Padukone-t2.jpg</t>
         </is>
       </c>
-      <c r="E108" t="inlineStr"/>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F108" t="inlineStr"/>
       <c r="G108" t="inlineStr">
         <is>
@@ -9515,7 +10051,11 @@
           <t>halfbody-handswaist.webp</t>
         </is>
       </c>
-      <c r="T108" t="inlineStr"/>
+      <c r="T108" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\Beautiful-Deepika-Padukone-t2.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -9536,7 +10076,11 @@
           <t>Beautiful-Deepika-Padukone-t3.jpg</t>
         </is>
       </c>
-      <c r="E109" t="inlineStr"/>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F109" t="inlineStr"/>
       <c r="G109" t="inlineStr"/>
       <c r="H109" t="inlineStr"/>
@@ -9583,7 +10127,11 @@
           <t>sitting.jpg</t>
         </is>
       </c>
-      <c r="T109" t="inlineStr"/>
+      <c r="T109" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\Beautiful-Deepika-Padukone-t3.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -9604,7 +10152,11 @@
           <t>Beautiful-Deepika-Padukone-t4.jpg</t>
         </is>
       </c>
-      <c r="E110" t="inlineStr"/>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F110" t="inlineStr">
         <is>
           <t>provocative</t>
@@ -9659,7 +10211,11 @@
           <t>3quarters-mediumshot2.png</t>
         </is>
       </c>
-      <c r="T110" t="inlineStr"/>
+      <c r="T110" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\Beautiful-Deepika-Padukone-t4.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -9680,7 +10236,11 @@
           <t>Belinda-t1.jfif</t>
         </is>
       </c>
-      <c r="E111" t="inlineStr"/>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F111" t="inlineStr"/>
       <c r="G111" t="inlineStr">
         <is>
@@ -9743,7 +10303,11 @@
           <t>kneed.jpg</t>
         </is>
       </c>
-      <c r="T111" t="inlineStr"/>
+      <c r="T111" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\Belinda-t1.jfif</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -9764,7 +10328,11 @@
           <t>Belinda-t2.jfif</t>
         </is>
       </c>
-      <c r="E112" t="inlineStr"/>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F112" t="inlineStr"/>
       <c r="G112" t="inlineStr">
         <is>
@@ -9827,7 +10395,11 @@
           <t>stand-sit.jpg</t>
         </is>
       </c>
-      <c r="T112" t="inlineStr"/>
+      <c r="T112" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\Belinda-t2.jfif</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -9848,7 +10420,11 @@
           <t>Belinda-t3.jfif</t>
         </is>
       </c>
-      <c r="E113" t="inlineStr"/>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F113" t="inlineStr">
         <is>
           <t>provocative</t>
@@ -9907,7 +10483,11 @@
           <t>3q-stand-legswide.jpeg</t>
         </is>
       </c>
-      <c r="T113" t="inlineStr"/>
+      <c r="T113" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\Belinda-t3.jfif</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -9928,7 +10508,11 @@
           <t>Belinda-t4.jfif</t>
         </is>
       </c>
-      <c r="E114" t="inlineStr"/>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F114" t="inlineStr">
         <is>
           <t>provocative</t>
@@ -9987,7 +10571,11 @@
           <t>3quarters-mediumshot.jpg</t>
         </is>
       </c>
-      <c r="T114" t="inlineStr"/>
+      <c r="T114" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\Belinda-t4.jfif</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -10008,7 +10596,11 @@
           <t>Belinda_Peregrin_Schull-t1.jpg</t>
         </is>
       </c>
-      <c r="E115" t="inlineStr"/>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F115" t="inlineStr">
         <is>
           <t>naughty</t>
@@ -10063,7 +10655,11 @@
           <t>handup-2.jpg</t>
         </is>
       </c>
-      <c r="T115" t="inlineStr"/>
+      <c r="T115" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\Belinda_Peregrin_Schull-t1.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -10084,7 +10680,11 @@
           <t>Belinda_Peregrin_Schull-t2.jpg</t>
         </is>
       </c>
-      <c r="E116" t="inlineStr"/>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F116" t="inlineStr">
         <is>
           <t>hot</t>
@@ -10139,7 +10739,11 @@
           <t>stand-profile-2.jpg</t>
         </is>
       </c>
-      <c r="T116" t="inlineStr"/>
+      <c r="T116" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\Belinda_Peregrin_Schull-t2.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -10160,7 +10764,11 @@
           <t>Belinda_Peregrin_Schull-t3.jpg</t>
         </is>
       </c>
-      <c r="E117" t="inlineStr"/>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F117" t="inlineStr">
         <is>
           <t>hot</t>
@@ -10223,7 +10831,11 @@
           <t>halfbody.jpg</t>
         </is>
       </c>
-      <c r="T117" t="inlineStr"/>
+      <c r="T117" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\Belinda_Peregrin_Schull-t3.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -10244,7 +10856,11 @@
           <t>Belinda_Peregrin_Schull-t4.jpg</t>
         </is>
       </c>
-      <c r="E118" t="inlineStr"/>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F118" t="inlineStr">
         <is>
           <t>in leather</t>
@@ -10307,7 +10923,11 @@
           <t>3quarters-mediumshotdown.jfif</t>
         </is>
       </c>
-      <c r="T118" t="inlineStr"/>
+      <c r="T118" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\Belinda_Peregrin_Schull-t4.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -10328,7 +10948,11 @@
           <t>BlancaMoreno-t1.jpg</t>
         </is>
       </c>
-      <c r="E119" t="inlineStr"/>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F119" t="inlineStr">
         <is>
           <t>naughty</t>
@@ -10387,7 +11011,11 @@
           <t>pop.png</t>
         </is>
       </c>
-      <c r="T119" t="inlineStr"/>
+      <c r="T119" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\BlancaMoreno-t1.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -10408,7 +11036,11 @@
           <t>BlancaMoreno-t2.jpg</t>
         </is>
       </c>
-      <c r="E120" t="inlineStr"/>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F120" t="inlineStr">
         <is>
           <t>sensual</t>
@@ -10471,7 +11103,11 @@
           <t>stretch.jpg</t>
         </is>
       </c>
-      <c r="T120" t="inlineStr"/>
+      <c r="T120" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\BlancaMoreno-t2.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -10492,7 +11128,11 @@
           <t>BlancaMoreno-t3.jpg</t>
         </is>
       </c>
-      <c r="E121" t="inlineStr"/>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F121" t="inlineStr">
         <is>
           <t>sensual</t>
@@ -10555,7 +11195,11 @@
           <t>straight-handsback.jpg</t>
         </is>
       </c>
-      <c r="T121" t="inlineStr"/>
+      <c r="T121" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\BlancaMoreno-t3.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -10576,7 +11220,11 @@
           <t>BlancaMoreno-t4.jpg</t>
         </is>
       </c>
-      <c r="E122" t="inlineStr"/>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F122" t="inlineStr"/>
       <c r="G122" t="inlineStr">
         <is>
@@ -10639,7 +11287,11 @@
           <t>stand.webp</t>
         </is>
       </c>
-      <c r="T122" t="inlineStr"/>
+      <c r="T122" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\BlancaMoreno-t4.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -10660,7 +11312,11 @@
           <t>Branta-t1.jpeg</t>
         </is>
       </c>
-      <c r="E123" t="inlineStr"/>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F123" t="inlineStr"/>
       <c r="G123" t="inlineStr"/>
       <c r="H123" t="inlineStr">
@@ -10723,7 +11379,11 @@
           <t>3q-stand.jpg</t>
         </is>
       </c>
-      <c r="T123" t="inlineStr"/>
+      <c r="T123" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\Branta-t1.jpeg</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -10744,7 +11404,11 @@
           <t>Branta-t2.jpeg</t>
         </is>
       </c>
-      <c r="E124" t="inlineStr"/>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F124" t="inlineStr">
         <is>
           <t>provocative</t>
@@ -10807,7 +11471,11 @@
           <t>pose.jpg</t>
         </is>
       </c>
-      <c r="T124" t="inlineStr"/>
+      <c r="T124" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\Branta-t2.jpeg</t>
+        </is>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -10828,7 +11496,11 @@
           <t>Branta-t3.jpeg</t>
         </is>
       </c>
-      <c r="E125" t="inlineStr"/>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F125" t="inlineStr">
         <is>
           <t>sensual</t>
@@ -10891,7 +11563,11 @@
           <t>halfbody.jpg</t>
         </is>
       </c>
-      <c r="T125" t="inlineStr"/>
+      <c r="T125" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\Branta-t3.jpeg</t>
+        </is>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -10912,7 +11588,11 @@
           <t>Branta-t4.jpeg</t>
         </is>
       </c>
-      <c r="E126" t="inlineStr"/>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F126" t="inlineStr">
         <is>
           <t>beautiful</t>
@@ -10979,7 +11659,11 @@
           <t>face.jpg</t>
         </is>
       </c>
-      <c r="T126" t="inlineStr"/>
+      <c r="T126" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\Branta-t4.jpeg</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -11000,7 +11684,11 @@
           <t>Brenda-t1.jpg</t>
         </is>
       </c>
-      <c r="E127" t="inlineStr"/>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F127" t="inlineStr"/>
       <c r="G127" t="inlineStr">
         <is>
@@ -11055,7 +11743,11 @@
           <t>arm-up.jpg</t>
         </is>
       </c>
-      <c r="T127" t="inlineStr"/>
+      <c r="T127" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\Brenda-t1.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -11076,7 +11768,11 @@
           <t>Brenda-t2.jpg</t>
         </is>
       </c>
-      <c r="E128" t="inlineStr"/>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F128" t="inlineStr">
         <is>
           <t>sensual</t>
@@ -11139,7 +11835,11 @@
           <t>sitting.jpg</t>
         </is>
       </c>
-      <c r="T128" t="inlineStr"/>
+      <c r="T128" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\Brenda-t2.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -11160,7 +11860,11 @@
           <t>Brenda-t3.jpg</t>
         </is>
       </c>
-      <c r="E129" t="inlineStr"/>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F129" t="inlineStr">
         <is>
           <t>provocative</t>
@@ -11219,7 +11923,11 @@
           <t>stand-lookup.jpg</t>
         </is>
       </c>
-      <c r="T129" t="inlineStr"/>
+      <c r="T129" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\Brenda-t3.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -11240,7 +11948,11 @@
           <t>Brenda-t4.jpg</t>
         </is>
       </c>
-      <c r="E130" t="inlineStr"/>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F130" t="inlineStr">
         <is>
           <t>in leather</t>
@@ -11307,7 +12019,11 @@
           <t>front-mediumshotdown2.png</t>
         </is>
       </c>
-      <c r="T130" t="inlineStr"/>
+      <c r="T130" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\Brenda-t4.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -11328,7 +12044,11 @@
           <t>BrendaVeronica-t1.jpg</t>
         </is>
       </c>
-      <c r="E131" t="inlineStr"/>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 'Cannot find any face in the reference image! Please upload another person image'</t>
+        </is>
+      </c>
       <c r="F131" t="inlineStr">
         <is>
           <t>naughty</t>
@@ -11412,7 +12132,11 @@
           <t>BrendaVeronica-t2.jpg</t>
         </is>
       </c>
-      <c r="E132" t="inlineStr"/>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F132" t="inlineStr">
         <is>
           <t>hot</t>
@@ -11479,7 +12203,11 @@
           <t>3quarters-mediumshot.jfif</t>
         </is>
       </c>
-      <c r="T132" t="inlineStr"/>
+      <c r="T132" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\BrendaVeronica-t2.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -11500,7 +12228,11 @@
           <t>BrendaVeronica-t3.jpg</t>
         </is>
       </c>
-      <c r="E133" t="inlineStr"/>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F133" t="inlineStr">
         <is>
           <t>sensual</t>
@@ -11567,7 +12299,11 @@
           <t>17.webp</t>
         </is>
       </c>
-      <c r="T133" t="inlineStr"/>
+      <c r="T133" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\BrendaVeronica-t3.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -11588,7 +12324,11 @@
           <t>BrendaVeronica-t4.jpg</t>
         </is>
       </c>
-      <c r="E134" t="inlineStr"/>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F134" t="inlineStr">
         <is>
           <t>sensual</t>
@@ -11647,7 +12387,11 @@
           <t>front.webp</t>
         </is>
       </c>
-      <c r="T134" t="inlineStr"/>
+      <c r="T134" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\BrendaVeronica-t4.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -11668,7 +12412,11 @@
           <t>CaroGil-t1.png</t>
         </is>
       </c>
-      <c r="E135" t="inlineStr"/>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F135" t="inlineStr"/>
       <c r="G135" t="inlineStr"/>
       <c r="H135" t="inlineStr"/>
@@ -11723,7 +12471,11 @@
           <t>spread.jpg</t>
         </is>
       </c>
-      <c r="T135" t="inlineStr"/>
+      <c r="T135" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\CaroGil-t1.png</t>
+        </is>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -11744,7 +12496,11 @@
           <t>CaroGil-t2.png</t>
         </is>
       </c>
-      <c r="E136" t="inlineStr"/>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F136" t="inlineStr">
         <is>
           <t>hot</t>
@@ -11799,7 +12555,11 @@
           <t>group.jpg</t>
         </is>
       </c>
-      <c r="T136" t="inlineStr"/>
+      <c r="T136" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\CaroGil-t2.png</t>
+        </is>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -11820,7 +12580,11 @@
           <t>CaroGil-t3.png</t>
         </is>
       </c>
-      <c r="E137" t="inlineStr"/>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F137" t="inlineStr"/>
       <c r="G137" t="inlineStr">
         <is>
@@ -11883,7 +12647,11 @@
           <t>stand-legsopen.jpg</t>
         </is>
       </c>
-      <c r="T137" t="inlineStr"/>
+      <c r="T137" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\CaroGil-t3.png</t>
+        </is>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -11904,7 +12672,11 @@
           <t>CaroGil-t4.png</t>
         </is>
       </c>
-      <c r="E138" t="inlineStr"/>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 'Cannot find any face in the reference image! Please upload another person image'</t>
+        </is>
+      </c>
       <c r="F138" t="inlineStr">
         <is>
           <t>hot</t>
@@ -11980,7 +12752,11 @@
           <t>ClauDrew-t1.jpg</t>
         </is>
       </c>
-      <c r="E139" t="inlineStr"/>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F139" t="inlineStr">
         <is>
           <t>in leather</t>
@@ -12043,7 +12819,11 @@
           <t>front-americanshot1.jpg</t>
         </is>
       </c>
-      <c r="T139" t="inlineStr"/>
+      <c r="T139" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\ClauDrew-t1.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -12064,7 +12844,11 @@
           <t>ClauDrew-t2.jpg</t>
         </is>
       </c>
-      <c r="E140" t="inlineStr"/>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F140" t="inlineStr">
         <is>
           <t>beautiful</t>
@@ -12123,7 +12907,11 @@
           <t>3quarters-mediumshotdown.webp</t>
         </is>
       </c>
-      <c r="T140" t="inlineStr"/>
+      <c r="T140" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\ClauDrew-t2.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -12144,7 +12932,11 @@
           <t>ClauDrew-t3.jpg</t>
         </is>
       </c>
-      <c r="E141" t="inlineStr"/>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F141" t="inlineStr">
         <is>
           <t>beautiful</t>
@@ -12211,7 +13003,11 @@
           <t>stand-takearm.jpg</t>
         </is>
       </c>
-      <c r="T141" t="inlineStr"/>
+      <c r="T141" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\ClauDrew-t3.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -12232,7 +13028,11 @@
           <t>ClauDrew-t4.jpg</t>
         </is>
       </c>
-      <c r="E142" t="inlineStr"/>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F142" t="inlineStr">
         <is>
           <t>naughty</t>
@@ -12295,7 +13095,11 @@
           <t>front-mediumshot5.png</t>
         </is>
       </c>
-      <c r="T142" t="inlineStr"/>
+      <c r="T142" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\ClauDrew-t4.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -12316,7 +13120,11 @@
           <t>Cougar-t1.png</t>
         </is>
       </c>
-      <c r="E143" t="inlineStr"/>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F143" t="inlineStr"/>
       <c r="G143" t="inlineStr">
         <is>
@@ -12371,7 +13179,11 @@
           <t>flying-pointing.jpg</t>
         </is>
       </c>
-      <c r="T143" t="inlineStr"/>
+      <c r="T143" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\Cougar-t1.png</t>
+        </is>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -12392,7 +13204,11 @@
           <t>Cougar-t2.png</t>
         </is>
       </c>
-      <c r="E144" t="inlineStr"/>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F144" t="inlineStr">
         <is>
           <t>in leather</t>
@@ -12455,7 +13271,11 @@
           <t>front-mediumshot3.png</t>
         </is>
       </c>
-      <c r="T144" t="inlineStr"/>
+      <c r="T144" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\Cougar-t2.png</t>
+        </is>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -12476,7 +13296,11 @@
           <t>Cougar-t3.png</t>
         </is>
       </c>
-      <c r="E145" t="inlineStr"/>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F145" t="inlineStr"/>
       <c r="G145" t="inlineStr">
         <is>
@@ -12531,7 +13355,11 @@
           <t>stand-sit.jpg</t>
         </is>
       </c>
-      <c r="T145" t="inlineStr"/>
+      <c r="T145" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\Cougar-t3.png</t>
+        </is>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -12552,7 +13380,11 @@
           <t>Cougar-t4.png</t>
         </is>
       </c>
-      <c r="E146" t="inlineStr"/>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F146" t="inlineStr">
         <is>
           <t>naughty</t>
@@ -12619,7 +13451,11 @@
           <t>front-medium-arms2.webp</t>
         </is>
       </c>
-      <c r="T146" t="inlineStr"/>
+      <c r="T146" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\Cougar-t4.png</t>
+        </is>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -12640,7 +13476,11 @@
           <t>DamarizGonzalez-t1.jpg</t>
         </is>
       </c>
-      <c r="E147" t="inlineStr"/>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F147" t="inlineStr">
         <is>
           <t>in leather</t>
@@ -12699,7 +13539,11 @@
           <t>handup.jpg</t>
         </is>
       </c>
-      <c r="T147" t="inlineStr"/>
+      <c r="T147" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\DamarizGonzalez-t1.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -12720,7 +13564,11 @@
           <t>DamarizGonzalez-t2.jpg</t>
         </is>
       </c>
-      <c r="E148" t="inlineStr"/>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F148" t="inlineStr"/>
       <c r="G148" t="inlineStr">
         <is>
@@ -12779,7 +13627,11 @@
           <t>front-mediumdownshot.png</t>
         </is>
       </c>
-      <c r="T148" t="inlineStr"/>
+      <c r="T148" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\DamarizGonzalez-t2.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -12800,7 +13652,11 @@
           <t>DamarizGonzalez-t3.jpg</t>
         </is>
       </c>
-      <c r="E149" t="inlineStr"/>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
       <c r="F149" t="inlineStr"/>
       <c r="G149" t="inlineStr">
         <is>
@@ -12863,7 +13719,11 @@
           <t>stand-far.jpg</t>
         </is>
       </c>
-      <c r="T149" t="inlineStr"/>
+      <c r="T149" t="inlineStr">
+        <is>
+          <t>D:\Dropbox\DevOps\Devs\NOW\hf-batcher\imagenes\resultados\girlsFull-results\DamarizGonzalez-t3.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">

</xml_diff>